<commit_message>
XML insert scripts into Staging
</commit_message>
<xml_diff>
--- a/Spreadsheet/FromLB/E I XML Mapping-SP_edits.xlsx
+++ b/Spreadsheet/FromLB/E I XML Mapping-SP_edits.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\source\repos\Solid Waste Migration\Spreadsheet\FromLB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\source\repos\solid-waste-migration\Spreadsheet\FromLB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC26688-D1C5-4255-ABA6-1CCEDE5DB0DA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39FBD6EE-B06B-4E02-A2F4-7877538EBB85}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="867" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19080" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="867" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="YTL" sheetId="1" r:id="rId1"/>
@@ -4698,7 +4698,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>77</v>
       </c>
@@ -4706,12 +4706,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>78</v>
       </c>
@@ -4730,7 +4730,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>81</v>
       </c>
@@ -4738,7 +4738,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>83</v>
       </c>
@@ -4746,7 +4746,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>84</v>
       </c>
@@ -4755,7 +4755,7 @@
       </c>
       <c r="C54" s="10"/>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>86</v>
       </c>
@@ -4763,7 +4763,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>88</v>
       </c>
@@ -4771,12 +4771,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
       <c r="B57" s="8"/>
       <c r="C57" s="8"/>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>89</v>
       </c>
@@ -4795,7 +4795,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>92</v>
       </c>
@@ -4803,7 +4803,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>94</v>
       </c>
@@ -4811,7 +4811,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>95</v>
       </c>
@@ -5492,19 +5492,19 @@
       </c>
       <c r="C39" s="17"/>
     </row>
-    <row r="40" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="18" t="s">
         <v>25</v>
       </c>
       <c r="B40" s="19"/>
       <c r="C40" s="20"/>
     </row>
-    <row r="41" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="21"/>
       <c r="B41" s="22"/>
       <c r="C41" s="23"/>
     </row>
-    <row r="42" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="18" t="s">
         <v>14</v>
       </c>
@@ -5513,7 +5513,7 @@
       </c>
       <c r="C42" s="20"/>
     </row>
-    <row r="43" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="27" t="s">
         <v>16</v>
       </c>
@@ -5524,7 +5524,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="18" t="s">
         <v>18</v>
       </c>
@@ -5533,7 +5533,7 @@
       </c>
       <c r="C44" s="20"/>
     </row>
-    <row r="45" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="27" t="s">
         <v>20</v>
       </c>
@@ -5542,7 +5542,7 @@
       </c>
       <c r="C45" s="17"/>
     </row>
-    <row r="46" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="18" t="s">
         <v>21</v>
       </c>
@@ -5551,7 +5551,7 @@
       </c>
       <c r="C46" s="24"/>
     </row>
-    <row r="47" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="27" t="s">
         <v>23</v>
       </c>
@@ -5560,19 +5560,19 @@
       </c>
       <c r="C47" s="17"/>
     </row>
-    <row r="48" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="18" t="s">
         <v>25</v>
       </c>
       <c r="B48" s="19"/>
       <c r="C48" s="20"/>
     </row>
-    <row r="49" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="21"/>
       <c r="B49" s="22"/>
       <c r="C49" s="23"/>
     </row>
-    <row r="50" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="18" t="s">
         <v>14</v>
       </c>
@@ -5581,7 +5581,7 @@
       </c>
       <c r="C50" s="20"/>
     </row>
-    <row r="51" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="27" t="s">
         <v>16</v>
       </c>
@@ -5592,7 +5592,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="18" t="s">
         <v>18</v>
       </c>
@@ -5601,7 +5601,7 @@
       </c>
       <c r="C52" s="20"/>
     </row>
-    <row r="53" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="27" t="s">
         <v>20</v>
       </c>
@@ -5610,7 +5610,7 @@
       </c>
       <c r="C53" s="17"/>
     </row>
-    <row r="54" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="18" t="s">
         <v>21</v>
       </c>
@@ -11063,7 +11063,7 @@
       </c>
       <c r="C22" s="9"/>
     </row>
-    <row r="23" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -11071,7 +11071,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -11079,12 +11079,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="7"/>
     </row>
-    <row r="26" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -11092,7 +11092,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -13010,12 +13010,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="7"/>
     </row>
-    <row r="26" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -13023,7 +13023,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -13034,7 +13034,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -13042,7 +13042,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -15478,8 +15478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:G231"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
@@ -17475,14 +17475,14 @@
   <dimension ref="A1:G164"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="A164" sqref="A164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.85546875" customWidth="1"/>
     <col min="2" max="2" width="52.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="165.140625" customWidth="1"/>
+    <col min="3" max="3" width="176" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
@@ -17698,7 +17698,7 @@
       <c r="F22" s="19"/>
       <c r="G22" s="24"/>
     </row>
-    <row r="23" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -17711,7 +17711,7 @@
       <c r="F23" s="16"/>
       <c r="G23" s="17"/>
     </row>
-    <row r="24" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -17724,12 +17724,12 @@
       <c r="F24" s="19"/>
       <c r="G24" s="20"/>
     </row>
-    <row r="25" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="7"/>
     </row>
-    <row r="26" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -17737,7 +17737,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -19105,7 +19105,7 @@
       </c>
       <c r="C22" s="9"/>
     </row>
-    <row r="23" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -19113,7 +19113,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -19121,12 +19121,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="7"/>
     </row>
-    <row r="26" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -19134,7 +19134,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -19755,7 +19755,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>63</v>
       </c>
@@ -19764,7 +19764,7 @@
       </c>
       <c r="C46" s="9"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>65</v>
       </c>
@@ -19772,7 +19772,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>67</v>
       </c>
@@ -19780,12 +19780,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
       <c r="B49" s="8"/>
       <c r="C49" s="7"/>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>68</v>
       </c>
@@ -20198,7 +20198,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>60</v>
       </c>
@@ -20206,7 +20206,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>62</v>
       </c>
@@ -20214,7 +20214,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>63</v>
       </c>
@@ -20223,7 +20223,7 @@
       </c>
       <c r="C38" s="9"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>65</v>
       </c>
@@ -20231,7 +20231,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>67</v>
       </c>
@@ -20239,12 +20239,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="8"/>
       <c r="C41" s="7"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>78</v>
       </c>
@@ -20252,7 +20252,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>80</v>
       </c>
@@ -20263,7 +20263,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>81</v>
       </c>
@@ -20271,7 +20271,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>83</v>
       </c>
@@ -20279,7 +20279,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>84</v>
       </c>
@@ -20288,7 +20288,7 @@
       </c>
       <c r="C46" s="9"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>86</v>
       </c>
@@ -20296,7 +20296,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>88</v>
       </c>
@@ -20304,12 +20304,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="21"/>
       <c r="B49" s="22"/>
       <c r="C49" s="23"/>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="18" t="s">
         <v>68</v>
       </c>
@@ -20832,12 +20832,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="21"/>
       <c r="B25" s="22"/>
       <c r="C25" s="23"/>
     </row>
-    <row r="26" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -20845,7 +20845,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -20856,7 +20856,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -20864,7 +20864,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -20872,7 +20872,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>45</v>
       </c>
@@ -20881,7 +20881,7 @@
       </c>
       <c r="C30" s="9"/>
     </row>
-    <row r="31" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>47</v>
       </c>
@@ -20889,7 +20889,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -20897,12 +20897,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="8"/>
       <c r="C33" s="7"/>
     </row>
-    <row r="34" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="36" t="s">
         <v>466</v>
       </c>
@@ -20910,7 +20910,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="25" t="s">
         <v>467</v>
       </c>
@@ -20921,7 +20921,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="36" t="s">
         <v>468</v>
       </c>
@@ -20929,7 +20929,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="25" t="s">
         <v>469</v>
       </c>
@@ -20937,7 +20937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="36" t="s">
         <v>470</v>
       </c>
@@ -20946,7 +20946,7 @@
       </c>
       <c r="C38" s="9"/>
     </row>
-    <row r="39" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="25" t="s">
         <v>471</v>
       </c>
@@ -22591,12 +22591,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="7"/>
     </row>
-    <row r="26" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -22604,7 +22604,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -22615,7 +22615,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -22623,7 +22623,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -23978,8 +23978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G164"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C99" sqref="C99"/>
     </sheetView>
   </sheetViews>
@@ -25669,12 +25669,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="7"/>
     </row>
-    <row r="26" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>50</v>
       </c>
@@ -25682,7 +25682,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>51</v>
       </c>
@@ -25693,7 +25693,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -25701,7 +25701,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>53</v>
       </c>
@@ -30176,7 +30176,7 @@
       </c>
       <c r="C22" s="9"/>
     </row>
-    <row r="23" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -30184,7 +30184,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -30192,12 +30192,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="7"/>
     </row>
-    <row r="26" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -30205,7 +30205,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -30216,7 +30216,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -30224,7 +30224,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -30232,7 +30232,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>45</v>
       </c>
@@ -30241,7 +30241,7 @@
       </c>
       <c r="C30" s="9"/>
     </row>
-    <row r="31" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>47</v>
       </c>
@@ -30249,7 +30249,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -30257,12 +30257,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="8"/>
       <c r="C33" s="7"/>
     </row>
-    <row r="34" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="25" t="s">
         <v>466</v>
       </c>
@@ -30270,7 +30270,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="25" t="s">
         <v>467</v>
       </c>
@@ -30281,7 +30281,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="25" t="s">
         <v>468</v>
       </c>
@@ -30289,7 +30289,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="25" t="s">
         <v>469</v>
       </c>
@@ -30297,7 +30297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="25" t="s">
         <v>470</v>
       </c>

</xml_diff>

<commit_message>
Finishing initial Staging inserts
</commit_message>
<xml_diff>
--- a/Spreadsheet/FromLB/E I XML Mapping-SP_edits.xlsx
+++ b/Spreadsheet/FromLB/E I XML Mapping-SP_edits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\source\repos\solid-waste-migration\Spreadsheet\FromLB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39FBD6EE-B06B-4E02-A2F4-7877538EBB85}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3503106B-DFBA-47F4-8DE5-10A2C832BD41}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19080" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="867" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="867" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="YTL" sheetId="1" r:id="rId1"/>
@@ -2254,9 +2254,6 @@
     <t>[dbo].[Construction].Cell(s) where [dbo].[Construction].MajorCode = 'Approved Site to Receive Waste' or 'Approval to Receive Waste' and [dbo].[Construction].MinorCode = 'Issued' or 'Approved' or 'Sent'</t>
   </si>
   <si>
-    <t>[dbo].[MAIN FACILITY INFO].[Type of Waste(s) Processed by MRF]</t>
-  </si>
-  <si>
     <t>[Closure].[Comments] where [Closure].[MajorCode]='Closure Certification' or 'Closure Certificate' or 'Partial Closure Acceptance Letter' and [Closure].[MinorCode]= 'Issued' or 'Sent'</t>
   </si>
   <si>
@@ -2295,6 +2292,9 @@
   </si>
   <si>
     <t>[dbo].[Modification].[MajorCode]+' --'+[dbo].[Modifications].[Comments]</t>
+  </si>
+  <si>
+    <t>[dbo].[MAIN FACILITY INFO].[Type of Waste(s) Processed by MRF] ---- No Migrate?</t>
   </si>
 </sst>
 </file>
@@ -2906,7 +2906,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2945,38 +2945,29 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2986,7 +2977,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2995,7 +2986,6 @@
     <xf numFmtId="0" fontId="14" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4727,7 +4717,7 @@
         <v>43423</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -4791,7 +4781,7 @@
       <c r="B59" s="2">
         <v>43431</v>
       </c>
-      <c r="C59" s="41" t="s">
+      <c r="C59" s="38" t="s">
         <v>443</v>
       </c>
     </row>
@@ -4857,7 +4847,7 @@
         <v>0</v>
       </c>
       <c r="C67" s="10" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -4922,8 +4912,8 @@
       <c r="B75" s="16">
         <v>1</v>
       </c>
-      <c r="C75" s="40" t="s">
-        <v>741</v>
+      <c r="C75" s="37" t="s">
+        <v>740</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -4970,9 +4960,9 @@
       <c r="C80" s="20"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="38"/>
-      <c r="B81" s="39"/>
-      <c r="C81" s="39"/>
+      <c r="A81" s="35"/>
+      <c r="B81" s="36"/>
+      <c r="C81" s="36"/>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
@@ -5154,7 +5144,7 @@
         <v>378</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
@@ -5452,7 +5442,7 @@
       <c r="B35" s="16">
         <v>250000</v>
       </c>
-      <c r="C35" s="40" t="s">
+      <c r="C35" s="37" t="s">
         <v>714</v>
       </c>
     </row>
@@ -5520,7 +5510,7 @@
       <c r="B43" s="16">
         <v>180000</v>
       </c>
-      <c r="C43" s="40" t="s">
+      <c r="C43" s="37" t="s">
         <v>715</v>
       </c>
     </row>
@@ -5588,7 +5578,7 @@
       <c r="B51" s="16">
         <v>6</v>
       </c>
-      <c r="C51" s="40" t="s">
+      <c r="C51" s="37" t="s">
         <v>716</v>
       </c>
     </row>
@@ -5656,7 +5646,7 @@
       <c r="B59" s="16">
         <v>10</v>
       </c>
-      <c r="C59" s="40" t="s">
+      <c r="C59" s="37" t="s">
         <v>717</v>
       </c>
     </row>
@@ -5724,7 +5714,7 @@
       <c r="B67" s="16">
         <v>10</v>
       </c>
-      <c r="C67" s="40" t="s">
+      <c r="C67" s="37" t="s">
         <v>718</v>
       </c>
     </row>
@@ -5855,8 +5845,8 @@
         <v>16</v>
       </c>
       <c r="B83" s="16"/>
-      <c r="C83" s="40" t="s">
-        <v>741</v>
+      <c r="C83" s="37" t="s">
+        <v>740</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -6249,7 +6239,7 @@
         <v>333</v>
       </c>
       <c r="C131" s="15" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -6379,8 +6369,8 @@
       <c r="B147" s="16" t="s">
         <v>612</v>
       </c>
-      <c r="C147" s="40" t="s">
-        <v>741</v>
+      <c r="C147" s="37" t="s">
+        <v>740</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
@@ -6447,7 +6437,7 @@
         <v>43406</v>
       </c>
       <c r="C155" s="15" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
@@ -6508,7 +6498,7 @@
       <c r="A163" t="s">
         <v>149</v>
       </c>
-      <c r="B163" s="30">
+      <c r="B163" s="1">
         <v>5</v>
       </c>
       <c r="C163" s="15" t="s">
@@ -6707,7 +6697,7 @@
         <v>587</v>
       </c>
       <c r="C187" s="15" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
@@ -6772,7 +6762,7 @@
         <v>587</v>
       </c>
       <c r="C195" s="15" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
@@ -6822,7 +6812,7 @@
       <c r="C201" s="7"/>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A202" s="33" t="s">
+      <c r="A202" s="30" t="s">
         <v>473</v>
       </c>
     </row>
@@ -6830,33 +6820,33 @@
       <c r="A203" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="B203" s="31">
+      <c r="B203" s="2">
         <v>43168</v>
       </c>
       <c r="C203" s="9" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="B204" s="32" t="s">
+      <c r="B204" s="1" t="s">
         <v>590</v>
       </c>
       <c r="C204" s="15" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="205" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="B205" s="31">
+      <c r="B205" s="2">
         <v>43255</v>
       </c>
-      <c r="C205" s="44" t="s">
-        <v>749</v>
+      <c r="C205" s="40" t="s">
+        <v>748</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
@@ -6865,7 +6855,7 @@
       <c r="C206" s="7"/>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A207" s="33" t="s">
+      <c r="A207" s="30" t="s">
         <v>477</v>
       </c>
     </row>
@@ -6908,7 +6898,7 @@
       <c r="C211" s="7"/>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A212" s="34" t="s">
+      <c r="A212" s="31" t="s">
         <v>481</v>
       </c>
     </row>
@@ -6919,7 +6909,7 @@
       <c r="B213" s="2">
         <v>43227</v>
       </c>
-      <c r="C213" s="43" t="s">
+      <c r="C213" s="39" t="s">
         <v>734</v>
       </c>
     </row>
@@ -6940,7 +6930,7 @@
       <c r="C215" s="7"/>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A216" s="34" t="s">
+      <c r="A216" s="31" t="s">
         <v>594</v>
       </c>
     </row>
@@ -6963,7 +6953,7 @@
         <v>43466</v>
       </c>
       <c r="C218" s="15" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
@@ -6974,7 +6964,7 @@
         <v>43830</v>
       </c>
       <c r="C219" s="15" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
@@ -7090,15 +7080,15 @@
   <dimension ref="A1:G220"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A179" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C67" sqref="C67"/>
+      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.85546875" customWidth="1"/>
-    <col min="2" max="2" width="68.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="2" max="2" width="67.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="65.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
@@ -7698,8 +7688,8 @@
       <c r="B67" s="16">
         <v>10</v>
       </c>
-      <c r="C67" s="40" t="s">
-        <v>741</v>
+      <c r="C67" s="37" t="s">
+        <v>740</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -7829,8 +7819,8 @@
         <v>16</v>
       </c>
       <c r="B83" s="16"/>
-      <c r="C83" s="40" t="s">
-        <v>741</v>
+      <c r="C83" s="37" t="s">
+        <v>740</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -7960,7 +7950,7 @@
         <v>16</v>
       </c>
       <c r="B99" s="16"/>
-      <c r="C99" s="42" t="s">
+      <c r="C99" s="24" t="s">
         <v>678</v>
       </c>
     </row>
@@ -8223,7 +8213,7 @@
         <v>333</v>
       </c>
       <c r="C131" s="15" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -8353,7 +8343,7 @@
         <v>43406</v>
       </c>
       <c r="C147" s="9" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
@@ -8414,7 +8404,7 @@
       <c r="A155" t="s">
         <v>149</v>
       </c>
-      <c r="B155" s="30">
+      <c r="B155" s="1">
         <v>5</v>
       </c>
       <c r="C155" s="9" t="s">
@@ -8613,7 +8603,7 @@
         <v>587</v>
       </c>
       <c r="C179" s="15" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
@@ -8678,7 +8668,7 @@
         <v>587</v>
       </c>
       <c r="C187" s="15" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
@@ -8728,7 +8718,7 @@
       <c r="C193" s="7"/>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A194" s="33" t="s">
+      <c r="A194" s="30" t="s">
         <v>473</v>
       </c>
     </row>
@@ -8736,33 +8726,33 @@
       <c r="A195" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="B195" s="31">
+      <c r="B195" s="2">
         <v>43168</v>
       </c>
       <c r="C195" s="9" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="B196" s="32" t="s">
+      <c r="B196" s="1" t="s">
         <v>590</v>
       </c>
       <c r="C196" s="15" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="B197" s="31">
+      <c r="B197" s="2">
         <v>43255</v>
       </c>
       <c r="C197" s="9" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
@@ -8771,7 +8761,7 @@
       <c r="C198" s="7"/>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A199" s="33" t="s">
+      <c r="A199" s="30" t="s">
         <v>477</v>
       </c>
     </row>
@@ -8814,7 +8804,7 @@
       <c r="C203" s="7"/>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A204" s="34" t="s">
+      <c r="A204" s="31" t="s">
         <v>481</v>
       </c>
     </row>
@@ -8825,7 +8815,7 @@
       <c r="B205" s="2">
         <v>43227</v>
       </c>
-      <c r="C205" s="43" t="s">
+      <c r="C205" s="39" t="s">
         <v>734</v>
       </c>
     </row>
@@ -8846,7 +8836,7 @@
       <c r="C207" s="7"/>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A208" s="34" t="s">
+      <c r="A208" s="31" t="s">
         <v>594</v>
       </c>
     </row>
@@ -8869,7 +8859,7 @@
         <v>43466</v>
       </c>
       <c r="C210" s="15" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
@@ -8880,7 +8870,7 @@
         <v>43830</v>
       </c>
       <c r="C211" s="15" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
@@ -8994,15 +8984,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:G212"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A179" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B172" sqref="B172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.28515625" customWidth="1"/>
-    <col min="2" max="2" width="84.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="75" style="1" customWidth="1"/>
     <col min="3" max="3" width="80.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9394,8 +9384,8 @@
         <v>16</v>
       </c>
       <c r="B43" s="16"/>
-      <c r="C43" s="40" t="s">
-        <v>745</v>
+      <c r="C43" s="37" t="s">
+        <v>744</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
@@ -9525,7 +9515,7 @@
         <v>16</v>
       </c>
       <c r="B59" s="16"/>
-      <c r="C59" s="42" t="s">
+      <c r="C59" s="24" t="s">
         <v>678</v>
       </c>
     </row>
@@ -9788,7 +9778,7 @@
         <v>13</v>
       </c>
       <c r="C91" s="15" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
@@ -10119,7 +10109,7 @@
         <v>651</v>
       </c>
       <c r="C131" s="15" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
@@ -10184,7 +10174,7 @@
         <v>653</v>
       </c>
       <c r="C139" s="15" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
@@ -10249,7 +10239,7 @@
         <v>657</v>
       </c>
       <c r="C147" s="15" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="148" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
@@ -10314,7 +10304,7 @@
         <v>563</v>
       </c>
       <c r="C155" s="15" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="156" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
@@ -10379,7 +10369,7 @@
         <v>563</v>
       </c>
       <c r="C163" s="15" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="164" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
@@ -10445,7 +10435,7 @@
         <v>10</v>
       </c>
       <c r="C171" s="15" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="172" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
@@ -10562,7 +10552,7 @@
       <c r="C185" s="7"/>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A186" s="33" t="s">
+      <c r="A186" s="30" t="s">
         <v>473</v>
       </c>
     </row>
@@ -10570,33 +10560,33 @@
       <c r="A187" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="B187" s="31">
+      <c r="B187" s="2">
         <v>43168</v>
       </c>
       <c r="C187" s="9" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="B188" s="32" t="s">
+      <c r="B188" s="1" t="s">
         <v>590</v>
       </c>
       <c r="C188" s="15" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="B189" s="31">
+      <c r="B189" s="2">
         <v>43255</v>
       </c>
       <c r="C189" s="9" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
@@ -10605,7 +10595,7 @@
       <c r="C190" s="7"/>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A191" s="33" t="s">
+      <c r="A191" s="30" t="s">
         <v>477</v>
       </c>
     </row>
@@ -10648,7 +10638,7 @@
       <c r="C195" s="7"/>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A196" s="34" t="s">
+      <c r="A196" s="31" t="s">
         <v>481</v>
       </c>
     </row>
@@ -10659,7 +10649,7 @@
       <c r="B197" s="2">
         <v>43227</v>
       </c>
-      <c r="C197" s="43" t="s">
+      <c r="C197" s="39" t="s">
         <v>734</v>
       </c>
     </row>
@@ -10680,7 +10670,7 @@
       <c r="C199" s="7"/>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A200" s="34" t="s">
+      <c r="A200" s="31" t="s">
         <v>594</v>
       </c>
     </row>
@@ -10703,7 +10693,7 @@
         <v>43466</v>
       </c>
       <c r="C202" s="15" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
@@ -10714,7 +10704,7 @@
         <v>43830</v>
       </c>
       <c r="C203" s="15" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
@@ -11437,8 +11427,8 @@
       <c r="B67" s="16">
         <v>10</v>
       </c>
-      <c r="C67" s="40" t="s">
-        <v>741</v>
+      <c r="C67" s="37" t="s">
+        <v>740</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -11568,8 +11558,8 @@
         <v>16</v>
       </c>
       <c r="B83" s="16"/>
-      <c r="C83" s="40" t="s">
-        <v>741</v>
+      <c r="C83" s="37" t="s">
+        <v>740</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -11699,7 +11689,7 @@
         <v>16</v>
       </c>
       <c r="B99" s="16"/>
-      <c r="C99" s="42" t="s">
+      <c r="C99" s="24" t="s">
         <v>678</v>
       </c>
     </row>
@@ -11962,7 +11952,7 @@
         <v>333</v>
       </c>
       <c r="C131" s="15" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -12092,7 +12082,7 @@
         <v>43406</v>
       </c>
       <c r="C147" s="9" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
@@ -12153,7 +12143,7 @@
       <c r="A155" t="s">
         <v>149</v>
       </c>
-      <c r="B155" s="30">
+      <c r="B155" s="1">
         <v>5</v>
       </c>
       <c r="C155" s="9" t="s">
@@ -12352,7 +12342,7 @@
         <v>587</v>
       </c>
       <c r="C179" s="15" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
@@ -12417,7 +12407,7 @@
         <v>587</v>
       </c>
       <c r="C187" s="15" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
@@ -12467,7 +12457,7 @@
       <c r="C193" s="7"/>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A194" s="33" t="s">
+      <c r="A194" s="30" t="s">
         <v>473</v>
       </c>
       <c r="B194" s="1"/>
@@ -12476,33 +12466,33 @@
       <c r="A195" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="B195" s="31">
+      <c r="B195" s="2">
         <v>43168</v>
       </c>
       <c r="C195" s="9" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="B196" s="32" t="s">
+      <c r="B196" s="1" t="s">
         <v>590</v>
       </c>
       <c r="C196" s="15" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="B197" s="31">
+      <c r="B197" s="2">
         <v>43255</v>
       </c>
       <c r="C197" s="9" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
@@ -12511,7 +12501,7 @@
       <c r="C198" s="7"/>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A199" s="33" t="s">
+      <c r="A199" s="30" t="s">
         <v>477</v>
       </c>
       <c r="B199" s="1"/>
@@ -12555,7 +12545,7 @@
       <c r="C203" s="7"/>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A204" s="34" t="s">
+      <c r="A204" s="31" t="s">
         <v>481</v>
       </c>
       <c r="B204" s="1"/>
@@ -12567,7 +12557,7 @@
       <c r="B205" s="2">
         <v>43227</v>
       </c>
-      <c r="C205" s="43" t="s">
+      <c r="C205" s="39" t="s">
         <v>734</v>
       </c>
     </row>
@@ -12588,7 +12578,7 @@
       <c r="C207" s="7"/>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A208" s="34" t="s">
+      <c r="A208" s="31" t="s">
         <v>594</v>
       </c>
       <c r="B208" s="1"/>
@@ -12612,7 +12602,7 @@
         <v>43466</v>
       </c>
       <c r="C210" s="15" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
@@ -12623,7 +12613,7 @@
         <v>43830</v>
       </c>
       <c r="C211" s="15" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
@@ -12760,8 +12750,8 @@
   <dimension ref="A1:G80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H43" sqref="H43"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13360,7 +13350,7 @@
       <c r="B67" s="1" t="s">
         <v>576</v>
       </c>
-      <c r="C67" s="41" t="s">
+      <c r="C67" s="38" t="s">
         <v>709</v>
       </c>
     </row>
@@ -13739,7 +13729,7 @@
       <c r="C25" s="7"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="34" t="s">
+      <c r="A26" s="31" t="s">
         <v>573</v>
       </c>
     </row>
@@ -13751,7 +13741,7 @@
         <v>565</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
@@ -13775,8 +13765,8 @@
       <c r="B30" s="16" t="s">
         <v>571</v>
       </c>
-      <c r="C30" s="40" t="s">
-        <v>741</v>
+      <c r="C30" s="37" t="s">
+        <v>740</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
@@ -14180,8 +14170,8 @@
       <c r="B78" s="16">
         <v>40</v>
       </c>
-      <c r="C78" s="40" t="s">
-        <v>741</v>
+      <c r="C78" s="37" t="s">
+        <v>740</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -14311,8 +14301,8 @@
         <v>16</v>
       </c>
       <c r="B94" s="16"/>
-      <c r="C94" s="40" t="s">
-        <v>741</v>
+      <c r="C94" s="37" t="s">
+        <v>740</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -14442,7 +14432,7 @@
         <v>16</v>
       </c>
       <c r="B110" s="16"/>
-      <c r="C110" s="42" t="s">
+      <c r="C110" s="24" t="s">
         <v>678</v>
       </c>
     </row>
@@ -14705,7 +14695,7 @@
         <v>13</v>
       </c>
       <c r="C142" s="15" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
@@ -14835,7 +14825,7 @@
         <v>43426</v>
       </c>
       <c r="C158" s="9" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
@@ -15095,7 +15085,7 @@
         <v>126</v>
       </c>
       <c r="C190" s="15" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
@@ -15160,7 +15150,7 @@
         <v>338</v>
       </c>
       <c r="C198" s="15" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
@@ -15210,11 +15200,11 @@
       <c r="C204" s="7"/>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A205" s="34" t="s">
+      <c r="A205" s="31" t="s">
         <v>473</v>
       </c>
-      <c r="B205" s="35"/>
-      <c r="C205" s="36"/>
+      <c r="B205" s="32"/>
+      <c r="C205" s="33"/>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
@@ -15224,7 +15214,7 @@
         <v>42762</v>
       </c>
       <c r="C206" s="9" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
@@ -15235,7 +15225,7 @@
         <v>597</v>
       </c>
       <c r="C207" s="15" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
@@ -15246,7 +15236,7 @@
         <v>43129</v>
       </c>
       <c r="C208" s="9" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
@@ -15255,7 +15245,7 @@
       <c r="C209" s="7"/>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A210" s="34" t="s">
+      <c r="A210" s="31" t="s">
         <v>477</v>
       </c>
     </row>
@@ -15298,7 +15288,7 @@
       <c r="C214" s="7"/>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A215" s="34" t="s">
+      <c r="A215" s="31" t="s">
         <v>481</v>
       </c>
     </row>
@@ -15309,7 +15299,7 @@
       <c r="B216" s="2">
         <v>43080</v>
       </c>
-      <c r="C216" s="43" t="s">
+      <c r="C216" s="39" t="s">
         <v>734</v>
       </c>
     </row>
@@ -15330,7 +15320,7 @@
       <c r="C218" s="7"/>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A219" s="34" t="s">
+      <c r="A219" s="31" t="s">
         <v>594</v>
       </c>
     </row>
@@ -15353,7 +15343,7 @@
         <v>43466</v>
       </c>
       <c r="C221" s="15" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
@@ -15364,7 +15354,7 @@
         <v>43830</v>
       </c>
       <c r="C222" s="15" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
@@ -15478,8 +15468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:G231"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
@@ -15750,8 +15740,8 @@
       <c r="B27" s="16" t="s">
         <v>548</v>
       </c>
-      <c r="C27" s="40" t="s">
-        <v>741</v>
+      <c r="C27" s="37" t="s">
+        <v>740</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
@@ -16155,8 +16145,8 @@
       <c r="B75" s="16">
         <v>15</v>
       </c>
-      <c r="C75" s="40" t="s">
-        <v>741</v>
+      <c r="C75" s="37" t="s">
+        <v>740</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -16288,8 +16278,8 @@
       <c r="B91" s="16" t="s">
         <v>508</v>
       </c>
-      <c r="C91" s="40" t="s">
-        <v>741</v>
+      <c r="C91" s="37" t="s">
+        <v>740</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -16419,7 +16409,7 @@
         <v>16</v>
       </c>
       <c r="B107" s="16"/>
-      <c r="C107" s="42" t="s">
+      <c r="C107" s="24" t="s">
         <v>678</v>
       </c>
     </row>
@@ -16682,7 +16672,7 @@
         <v>13</v>
       </c>
       <c r="C139" s="15" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
@@ -16812,7 +16802,7 @@
         <v>43406</v>
       </c>
       <c r="C155" s="9" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
@@ -17072,7 +17062,7 @@
         <v>126</v>
       </c>
       <c r="C187" s="15" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
@@ -17137,7 +17127,7 @@
         <v>126</v>
       </c>
       <c r="C195" s="15" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
@@ -17187,11 +17177,11 @@
       <c r="C201" s="7"/>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A202" s="34" t="s">
+      <c r="A202" s="31" t="s">
         <v>594</v>
       </c>
-      <c r="B202" s="35"/>
-      <c r="C202" s="36"/>
+      <c r="B202" s="32"/>
+      <c r="C202" s="33"/>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
@@ -17331,10 +17321,10 @@
       <c r="C215" s="7"/>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A216" s="34" t="s">
+      <c r="A216" s="31" t="s">
         <v>473</v>
       </c>
-      <c r="C216" s="36"/>
+      <c r="C216" s="33"/>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
@@ -17375,13 +17365,13 @@
       <c r="C220" s="7"/>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A221" s="34" t="s">
+      <c r="A221" s="31" t="s">
         <v>399</v>
       </c>
       <c r="C221" s="25"/>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A222" s="36" t="s">
+      <c r="A222" s="33" t="s">
         <v>596</v>
       </c>
       <c r="B222" s="1" t="s">
@@ -17397,11 +17387,11 @@
       <c r="C223" s="7"/>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A224" s="34" t="s">
+      <c r="A224" s="31" t="s">
         <v>477</v>
       </c>
-      <c r="B224" s="35"/>
-      <c r="C224" s="36"/>
+      <c r="B224" s="32"/>
+      <c r="C224" s="33"/>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
@@ -17442,7 +17432,7 @@
       <c r="C228" s="7"/>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A229" s="34" t="s">
+      <c r="A229" s="31" t="s">
         <v>481</v>
       </c>
     </row>
@@ -17941,8 +17931,8 @@
         <v>16</v>
       </c>
       <c r="B51" s="16"/>
-      <c r="C51" s="40" t="s">
-        <v>741</v>
+      <c r="C51" s="37" t="s">
+        <v>740</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -18072,7 +18062,7 @@
         <v>16</v>
       </c>
       <c r="B67" s="16"/>
-      <c r="C67" s="42" t="s">
+      <c r="C67" s="24" t="s">
         <v>678</v>
       </c>
     </row>
@@ -18335,7 +18325,7 @@
         <v>13</v>
       </c>
       <c r="C99" s="15" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -18465,7 +18455,7 @@
         <v>43412</v>
       </c>
       <c r="C115" s="9" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -18530,7 +18520,7 @@
         <v>521</v>
       </c>
       <c r="C123" s="15" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -18645,11 +18635,11 @@
       <c r="C137" s="7"/>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138" s="34" t="s">
+      <c r="A138" s="31" t="s">
         <v>473</v>
       </c>
-      <c r="B138" s="35"/>
-      <c r="C138" s="36"/>
+      <c r="B138" s="32"/>
+      <c r="C138" s="33"/>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
@@ -18659,7 +18649,7 @@
         <v>42978</v>
       </c>
       <c r="C139" s="9" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
@@ -18670,7 +18660,7 @@
         <v>525</v>
       </c>
       <c r="C140" s="15" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
@@ -18681,7 +18671,7 @@
         <v>43010</v>
       </c>
       <c r="C141" s="9" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
@@ -18690,7 +18680,7 @@
       <c r="C142" s="7"/>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A143" s="34" t="s">
+      <c r="A143" s="31" t="s">
         <v>477</v>
       </c>
       <c r="B143" s="2"/>
@@ -18735,10 +18725,10 @@
       <c r="C147" s="7"/>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A148" s="34" t="s">
+      <c r="A148" s="31" t="s">
         <v>481</v>
       </c>
-      <c r="C148" s="36"/>
+      <c r="C148" s="33"/>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
@@ -18748,7 +18738,7 @@
         <v>42887</v>
       </c>
       <c r="C149" s="15" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
@@ -18759,7 +18749,7 @@
         <v>532</v>
       </c>
       <c r="C150" s="15" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
@@ -18768,10 +18758,10 @@
       <c r="C151" s="7"/>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A152" s="34" t="s">
+      <c r="A152" s="31" t="s">
         <v>594</v>
       </c>
-      <c r="C152" s="36"/>
+      <c r="C152" s="33"/>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
@@ -18792,7 +18782,7 @@
         <v>43472</v>
       </c>
       <c r="C154" s="15" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
@@ -18803,7 +18793,7 @@
         <v>43831</v>
       </c>
       <c r="C155" s="15" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
@@ -18915,8 +18905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19385,8 +19375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20903,7 +20893,7 @@
       <c r="C33" s="7"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="36" t="s">
+      <c r="A34" s="33" t="s">
         <v>466</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -20922,7 +20912,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="36" t="s">
+      <c r="A36" s="33" t="s">
         <v>468</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -20938,7 +20928,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="36" t="s">
+      <c r="A38" s="33" t="s">
         <v>470</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -20965,7 +20955,7 @@
       <c r="C41" s="7"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="36" t="s">
+      <c r="A42" s="33" t="s">
         <v>466</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -20984,7 +20974,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="36" t="s">
+      <c r="A44" s="33" t="s">
         <v>468</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -21000,7 +20990,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="36" t="s">
+      <c r="A46" s="33" t="s">
         <v>470</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -21107,8 +21097,8 @@
       <c r="B59" s="16" t="s">
         <v>508</v>
       </c>
-      <c r="C59" s="40" t="s">
-        <v>745</v>
+      <c r="C59" s="37" t="s">
+        <v>744</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -21240,7 +21230,7 @@
       <c r="B75" s="16" t="s">
         <v>513</v>
       </c>
-      <c r="C75" s="42" t="s">
+      <c r="C75" s="24" t="s">
         <v>678</v>
       </c>
     </row>
@@ -21372,7 +21362,7 @@
       <c r="B91" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C91" s="43" t="s">
+      <c r="C91" s="39" t="s">
         <v>680</v>
       </c>
     </row>
@@ -21437,7 +21427,7 @@
       <c r="B99" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C99" s="43" t="s">
+      <c r="C99" s="39" t="s">
         <v>681</v>
       </c>
     </row>
@@ -21502,8 +21492,8 @@
       <c r="B107" s="1">
         <v>2</v>
       </c>
-      <c r="C107" s="43" t="s">
-        <v>741</v>
+      <c r="C107" s="39" t="s">
+        <v>740</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -21828,7 +21818,7 @@
         <v>219</v>
       </c>
       <c r="C147" s="15" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
@@ -21958,7 +21948,7 @@
         <v>126</v>
       </c>
       <c r="C163" s="15" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
@@ -22023,7 +22013,7 @@
         <v>310</v>
       </c>
       <c r="C171" s="15" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
@@ -22073,7 +22063,7 @@
       <c r="C177" s="7"/>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A178" s="34" t="s">
+      <c r="A178" s="31" t="s">
         <v>473</v>
       </c>
     </row>
@@ -22085,7 +22075,7 @@
         <v>43098</v>
       </c>
       <c r="C179" s="9" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
@@ -22096,7 +22086,7 @@
         <v>484</v>
       </c>
       <c r="C180" s="15" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
@@ -22107,7 +22097,7 @@
         <v>43108</v>
       </c>
       <c r="C181" s="9" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
@@ -22116,7 +22106,7 @@
       <c r="C182" s="7"/>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A183" s="34" t="s">
+      <c r="A183" s="31" t="s">
         <v>477</v>
       </c>
     </row>
@@ -22159,7 +22149,7 @@
       <c r="C187" s="7"/>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A188" s="34" t="s">
+      <c r="A188" s="31" t="s">
         <v>481</v>
       </c>
     </row>
@@ -22170,7 +22160,7 @@
       <c r="B189" s="2">
         <v>42828</v>
       </c>
-      <c r="C189" s="43" t="s">
+      <c r="C189" s="39" t="s">
         <v>734</v>
       </c>
     </row>
@@ -22191,7 +22181,7 @@
       <c r="C191" s="7"/>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A192" s="34" t="s">
+      <c r="A192" s="31" t="s">
         <v>594</v>
       </c>
     </row>
@@ -22214,7 +22204,7 @@
         <v>43466</v>
       </c>
       <c r="C194" s="15" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
@@ -22225,7 +22215,7 @@
         <v>43830</v>
       </c>
       <c r="C195" s="15" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
@@ -22341,8 +22331,8 @@
   <dimension ref="A1:G188"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C163" sqref="C163:C165"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22662,7 +22652,7 @@
       <c r="C33" s="7"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="36" t="s">
+      <c r="A34" s="33" t="s">
         <v>466</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -22681,7 +22671,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="36" t="s">
+      <c r="A36" s="33" t="s">
         <v>468</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -22697,7 +22687,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="36" t="s">
+      <c r="A38" s="33" t="s">
         <v>470</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -22739,8 +22729,8 @@
       <c r="B43" s="16" t="s">
         <v>637</v>
       </c>
-      <c r="C43" s="40" t="s">
-        <v>741</v>
+      <c r="C43" s="37" t="s">
+        <v>740</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -22808,7 +22798,7 @@
         <v>587</v>
       </c>
       <c r="C51" s="24" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -22940,8 +22930,8 @@
       <c r="B67" s="16" t="s">
         <v>508</v>
       </c>
-      <c r="C67" s="40" t="s">
-        <v>745</v>
+      <c r="C67" s="37" t="s">
+        <v>744</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -23073,7 +23063,7 @@
       <c r="B83" s="16" t="s">
         <v>513</v>
       </c>
-      <c r="C83" s="40" t="s">
+      <c r="C83" s="37" t="s">
         <v>678</v>
       </c>
     </row>
@@ -23336,7 +23326,7 @@
         <v>2</v>
       </c>
       <c r="C115" s="15" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -23466,7 +23456,7 @@
         <v>43414</v>
       </c>
       <c r="C131" s="9" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -23531,7 +23521,7 @@
         <v>219</v>
       </c>
       <c r="C139" s="15" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
@@ -23661,7 +23651,7 @@
         <v>126</v>
       </c>
       <c r="C155" s="15" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
@@ -23711,7 +23701,7 @@
       <c r="C161" s="7"/>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A162" s="34" t="s">
+      <c r="A162" s="31" t="s">
         <v>473</v>
       </c>
     </row>
@@ -23723,7 +23713,7 @@
         <v>43098</v>
       </c>
       <c r="C163" s="9" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
@@ -23734,7 +23724,7 @@
         <v>484</v>
       </c>
       <c r="C164" s="15" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
@@ -23745,7 +23735,7 @@
         <v>43108</v>
       </c>
       <c r="C165" s="9" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
@@ -23754,7 +23744,7 @@
       <c r="C166" s="7"/>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A167" s="34" t="s">
+      <c r="A167" s="31" t="s">
         <v>477</v>
       </c>
     </row>
@@ -23797,7 +23787,7 @@
       <c r="C171" s="7"/>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A172" s="34" t="s">
+      <c r="A172" s="31" t="s">
         <v>481</v>
       </c>
     </row>
@@ -23808,7 +23798,7 @@
       <c r="B173" s="2">
         <v>42828</v>
       </c>
-      <c r="C173" s="43" t="s">
+      <c r="C173" s="39" t="s">
         <v>734</v>
       </c>
     </row>
@@ -23829,7 +23819,7 @@
       <c r="C175" s="7"/>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A176" s="34" t="s">
+      <c r="A176" s="31" t="s">
         <v>594</v>
       </c>
     </row>
@@ -23852,7 +23842,7 @@
         <v>43466</v>
       </c>
       <c r="C178" s="15" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
@@ -23863,7 +23853,7 @@
         <v>43830</v>
       </c>
       <c r="C179" s="15" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
@@ -24300,7 +24290,7 @@
       <c r="C33" s="7"/>
     </row>
     <row r="34" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A34" s="36" t="s">
+      <c r="A34" s="33" t="s">
         <v>466</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -24319,7 +24309,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A36" s="36" t="s">
+      <c r="A36" s="33" t="s">
         <v>468</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -24335,7 +24325,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A38" s="36" t="s">
+      <c r="A38" s="33" t="s">
         <v>470</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -24427,7 +24417,7 @@
       <c r="C49" s="23"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="37" t="s">
+      <c r="A50" s="34" t="s">
         <v>466</v>
       </c>
       <c r="B50" s="19" t="s">
@@ -24442,12 +24432,12 @@
       <c r="B51" s="16" t="s">
         <v>508</v>
       </c>
-      <c r="C51" s="40" t="s">
+      <c r="C51" s="37" t="s">
         <v>677</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="37" t="s">
+      <c r="A52" s="34" t="s">
         <v>468</v>
       </c>
       <c r="B52" s="19" t="s">
@@ -24465,7 +24455,7 @@
       <c r="C53" s="17"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="37" t="s">
+      <c r="A54" s="34" t="s">
         <v>470</v>
       </c>
       <c r="B54" s="19" t="s">
@@ -24560,7 +24550,7 @@
       <c r="C65" s="23"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="37" t="s">
+      <c r="A66" s="34" t="s">
         <v>466</v>
       </c>
       <c r="B66" s="19" t="s">
@@ -24575,12 +24565,12 @@
       <c r="B67" s="16" t="s">
         <v>513</v>
       </c>
-      <c r="C67" s="42" t="s">
+      <c r="C67" s="24" t="s">
         <v>678</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="37" t="s">
+      <c r="A68" s="34" t="s">
         <v>468</v>
       </c>
       <c r="B68" s="19" t="s">
@@ -24598,7 +24588,7 @@
       <c r="C69" s="17"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="37" t="s">
+      <c r="A70" s="34" t="s">
         <v>470</v>
       </c>
       <c r="B70" s="19" t="s">
@@ -24707,7 +24697,7 @@
       <c r="B83" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C83" s="43" t="s">
+      <c r="C83" s="39" t="s">
         <v>680</v>
       </c>
     </row>
@@ -24772,7 +24762,7 @@
       <c r="B91" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C91" s="43" t="s">
+      <c r="C91" s="39" t="s">
         <v>681</v>
       </c>
     </row>
@@ -25148,7 +25138,7 @@
       <c r="C137" s="7"/>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138" s="34" t="s">
+      <c r="A138" s="31" t="s">
         <v>473</v>
       </c>
     </row>
@@ -25191,7 +25181,7 @@
       <c r="C142" s="7"/>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A143" s="34" t="s">
+      <c r="A143" s="31" t="s">
         <v>477</v>
       </c>
     </row>
@@ -25234,7 +25224,7 @@
       <c r="C147" s="7"/>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A148" s="34" t="s">
+      <c r="A148" s="31" t="s">
         <v>481</v>
       </c>
     </row>
@@ -25266,7 +25256,7 @@
       <c r="C151" s="7"/>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A152" s="34" t="s">
+      <c r="A152" s="31" t="s">
         <v>594</v>
       </c>
     </row>
@@ -25420,7 +25410,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26144,7 +26134,7 @@
       <c r="B83" s="1">
         <v>3</v>
       </c>
-      <c r="C83" s="41" t="s">
+      <c r="C83" s="38" t="s">
         <v>707</v>
       </c>
     </row>
@@ -26333,8 +26323,8 @@
   <dimension ref="A1:G220"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A170" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C195" sqref="C195:C197"/>
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B89" sqref="B89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26616,7 +26606,7 @@
       <c r="C33" s="7"/>
     </row>
     <row r="34" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A34" s="36" t="s">
+      <c r="A34" s="33" t="s">
         <v>466</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -26635,7 +26625,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A36" s="36" t="s">
+      <c r="A36" s="33" t="s">
         <v>468</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -26651,7 +26641,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A38" s="36" t="s">
+      <c r="A38" s="33" t="s">
         <v>470</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -26678,7 +26668,7 @@
       <c r="C41" s="7"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="36" t="s">
+      <c r="A42" s="33" t="s">
         <v>466</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -26697,7 +26687,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="36" t="s">
+      <c r="A44" s="33" t="s">
         <v>468</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -26713,7 +26703,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="36" t="s">
+      <c r="A46" s="33" t="s">
         <v>470</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -26740,7 +26730,7 @@
       <c r="C49" s="7"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="36" t="s">
+      <c r="A50" s="33" t="s">
         <v>466</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -26759,7 +26749,7 @@
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="36" t="s">
+      <c r="A52" s="33" t="s">
         <v>468</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -26775,7 +26765,7 @@
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="36" t="s">
+      <c r="A54" s="33" t="s">
         <v>470</v>
       </c>
       <c r="B54" s="1" t="s">
@@ -26802,7 +26792,7 @@
       <c r="C57" s="7"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="36" t="s">
+      <c r="A58" s="33" t="s">
         <v>466</v>
       </c>
       <c r="B58" s="1" t="s">
@@ -26821,7 +26811,7 @@
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="36" t="s">
+      <c r="A60" s="33" t="s">
         <v>468</v>
       </c>
       <c r="B60" s="1" t="s">
@@ -26837,7 +26827,7 @@
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="36" t="s">
+      <c r="A62" s="33" t="s">
         <v>470</v>
       </c>
       <c r="B62" s="1" t="s">
@@ -26879,7 +26869,7 @@
         <v>30</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -27006,8 +26996,8 @@
       <c r="B83" s="16" t="s">
         <v>675</v>
       </c>
-      <c r="C83" s="40" t="s">
-        <v>741</v>
+      <c r="C83" s="37" t="s">
+        <v>740</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -27402,7 +27392,7 @@
         <v>2</v>
       </c>
       <c r="C131" s="15" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -27532,7 +27522,7 @@
         <v>43414</v>
       </c>
       <c r="C147" s="9" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
@@ -27830,7 +27820,7 @@
         <v>126</v>
       </c>
       <c r="C179" s="15" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
@@ -27895,7 +27885,7 @@
         <v>310</v>
       </c>
       <c r="C187" s="15" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
@@ -27945,7 +27935,7 @@
       <c r="C193" s="7"/>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A194" s="34" t="s">
+      <c r="A194" s="31" t="s">
         <v>473</v>
       </c>
     </row>
@@ -27957,7 +27947,7 @@
         <v>43098</v>
       </c>
       <c r="C195" s="9" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
@@ -27968,7 +27958,7 @@
         <v>484</v>
       </c>
       <c r="C196" s="15" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
@@ -27979,7 +27969,7 @@
         <v>43108</v>
       </c>
       <c r="C197" s="9" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
@@ -27988,7 +27978,7 @@
       <c r="C198" s="7"/>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A199" s="34" t="s">
+      <c r="A199" s="31" t="s">
         <v>477</v>
       </c>
     </row>
@@ -28031,7 +28021,7 @@
       <c r="C203" s="7"/>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A204" s="34" t="s">
+      <c r="A204" s="31" t="s">
         <v>481</v>
       </c>
     </row>
@@ -28042,7 +28032,7 @@
       <c r="B205" s="2">
         <v>42828</v>
       </c>
-      <c r="C205" s="43" t="s">
+      <c r="C205" s="39" t="s">
         <v>734</v>
       </c>
     </row>
@@ -28063,7 +28053,7 @@
       <c r="C207" s="7"/>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A208" s="34" t="s">
+      <c r="A208" s="31" t="s">
         <v>594</v>
       </c>
     </row>
@@ -28086,7 +28076,7 @@
         <v>43466</v>
       </c>
       <c r="C210" s="15" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
@@ -28097,7 +28087,7 @@
         <v>43830</v>
       </c>
       <c r="C211" s="15" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
@@ -28212,8 +28202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:H204"/>
   <sheetViews>
-    <sheetView topLeftCell="A166" workbookViewId="0">
-      <selection activeCell="C179" sqref="C179:C181"/>
+    <sheetView topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="B164" sqref="B164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28737,7 +28727,7 @@
       <c r="B59" s="16" t="s">
         <v>508</v>
       </c>
-      <c r="C59" s="40" t="s">
+      <c r="C59" s="37" t="s">
         <v>730</v>
       </c>
     </row>
@@ -28870,7 +28860,7 @@
       <c r="B75" s="16" t="s">
         <v>513</v>
       </c>
-      <c r="C75" s="42" t="s">
+      <c r="C75" s="24" t="s">
         <v>678</v>
       </c>
     </row>
@@ -29002,7 +28992,7 @@
       <c r="B91" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C91" s="43" t="s">
+      <c r="C91" s="39" t="s">
         <v>680</v>
       </c>
     </row>
@@ -29067,7 +29057,7 @@
       <c r="B99" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C99" s="43" t="s">
+      <c r="C99" s="39" t="s">
         <v>681</v>
       </c>
     </row>
@@ -29461,7 +29451,7 @@
         <v>346</v>
       </c>
       <c r="C147" s="14" t="s">
-        <v>738</v>
+        <v>751</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
@@ -29712,7 +29702,7 @@
       <c r="C177" s="7"/>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A178" s="33" t="s">
+      <c r="A178" s="30" t="s">
         <v>473</v>
       </c>
     </row>
@@ -29720,33 +29710,33 @@
       <c r="A179" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="B179" s="31">
+      <c r="B179" s="2">
         <v>43168</v>
       </c>
       <c r="C179" s="9" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="B180" s="32" t="s">
+      <c r="B180" s="1" t="s">
         <v>632</v>
       </c>
       <c r="C180" s="15" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="B181" s="31">
+      <c r="B181" s="2">
         <v>43255</v>
       </c>
       <c r="C181" s="9" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
@@ -29755,7 +29745,7 @@
       <c r="C182" s="7"/>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A183" s="33" t="s">
+      <c r="A183" s="30" t="s">
         <v>477</v>
       </c>
     </row>
@@ -29798,7 +29788,7 @@
       <c r="C187" s="7"/>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A188" s="34" t="s">
+      <c r="A188" s="31" t="s">
         <v>481</v>
       </c>
     </row>
@@ -29809,7 +29799,7 @@
       <c r="B189" s="2">
         <v>43227</v>
       </c>
-      <c r="C189" s="43" t="s">
+      <c r="C189" s="39" t="s">
         <v>734</v>
       </c>
     </row>
@@ -29830,7 +29820,7 @@
       <c r="C191" s="7"/>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A192" s="34" t="s">
+      <c r="A192" s="31" t="s">
         <v>594</v>
       </c>
     </row>
@@ -29853,7 +29843,7 @@
         <v>43466</v>
       </c>
       <c r="C194" s="15" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
@@ -29864,7 +29854,7 @@
         <v>43830</v>
       </c>
       <c r="C195" s="15" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
@@ -29979,8 +29969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G232"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B209" sqref="B209"/>
+    <sheetView topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="B172" sqref="B172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30564,7 +30554,7 @@
         <v>30</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -30691,8 +30681,8 @@
       <c r="B83" s="16" t="s">
         <v>508</v>
       </c>
-      <c r="C83" s="40" t="s">
-        <v>741</v>
+      <c r="C83" s="37" t="s">
+        <v>740</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -30824,7 +30814,7 @@
       <c r="B99" s="16" t="s">
         <v>513</v>
       </c>
-      <c r="C99" s="42" t="s">
+      <c r="C99" s="24" t="s">
         <v>678</v>
       </c>
     </row>
@@ -31087,7 +31077,7 @@
         <v>2</v>
       </c>
       <c r="C131" s="15" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -31217,7 +31207,7 @@
         <v>43414</v>
       </c>
       <c r="C147" s="9" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
@@ -31412,7 +31402,7 @@
         <v>219</v>
       </c>
       <c r="C171" s="15" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
@@ -31542,7 +31532,7 @@
         <v>126</v>
       </c>
       <c r="C187" s="15" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
@@ -31607,7 +31597,7 @@
         <v>310</v>
       </c>
       <c r="C195" s="15" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
@@ -31657,7 +31647,7 @@
       <c r="C201" s="7"/>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A202" s="34" t="s">
+      <c r="A202" s="31" t="s">
         <v>473</v>
       </c>
     </row>
@@ -31669,7 +31659,7 @@
         <v>42961</v>
       </c>
       <c r="C203" s="9" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
@@ -31680,7 +31670,7 @@
         <v>485</v>
       </c>
       <c r="C204" s="15" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
@@ -31691,7 +31681,7 @@
         <v>42944</v>
       </c>
       <c r="C205" s="9" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
@@ -31700,7 +31690,7 @@
       <c r="C206" s="7"/>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A207" s="34" t="s">
+      <c r="A207" s="31" t="s">
         <v>477</v>
       </c>
     </row>
@@ -31743,7 +31733,7 @@
       <c r="C211" s="7"/>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A212" s="34" t="s">
+      <c r="A212" s="31" t="s">
         <v>481</v>
       </c>
     </row>
@@ -31775,7 +31765,7 @@
       <c r="C215" s="7"/>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A216" s="34" t="s">
+      <c r="A216" s="31" t="s">
         <v>481</v>
       </c>
     </row>
@@ -31786,7 +31776,7 @@
       <c r="B217" s="2">
         <v>42927</v>
       </c>
-      <c r="C217" s="43" t="s">
+      <c r="C217" s="39" t="s">
         <v>734</v>
       </c>
     </row>
@@ -31807,7 +31797,7 @@
       <c r="C219" s="7"/>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A220" s="34" t="s">
+      <c r="A220" s="31" t="s">
         <v>594</v>
       </c>
     </row>
@@ -31830,7 +31820,7 @@
         <v>43466</v>
       </c>
       <c r="C222" s="15" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
@@ -31841,7 +31831,7 @@
         <v>43830</v>
       </c>
       <c r="C223" s="15" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>